<commit_message>
Fixes to unicode errors
</commit_message>
<xml_diff>
--- a/revised_reproduction_package_for_gaikwad_nellis(2021)/dataverse_files/exhibit-literature-review.xlsx
+++ b/revised_reproduction_package_for_gaikwad_nellis(2021)/dataverse_files/exhibit-literature-review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhargaikwad/Dropbox/Maitri/Replication/for-release/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamyayadav/Documents/GitHub/gaikwad_nellis_reproduction/revised_reproduction_package_for_gaikwad_nellis(2021)/dataverse_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67636F0-472C-694B-914A-63909C1A95D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F27A86-CE1E-384B-B570-F1BF4A392B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="3200" windowWidth="28800" windowHeight="16720" xr2:uid="{31725F55-5007-4EE2-98E0-28ABBB574EA6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{31725F55-5007-4EE2-98E0-28ABBB574EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,10 +234,6 @@
     <t>France, 2012 elections.  20,500 households across 10 cities, effect then studied as effect of registrations among those initially unregistered or misregistered. 1,500 households resampled for post-election survey.</t>
   </si>
   <si>
-    <t>Compared to registered voters as a whole, subjects who registered because of the treatment were more likely to be immigrants (+0.202, p&lt;0.01); born in another region of France (+0.215, p&lt;0.01); or young (age coefficient −0.137, p&lt;0.01). \newline \newline
-Voters registered from the treatments had higher turnout in the more salient  presidential election.</t>
-  </si>
-  <si>
     <t>U.S., 2012 in the months before the 2012 general election. 6,280 eligible but unregistered formerly incarcerated felons.</t>
   </si>
   <si>
@@ -325,6 +321,10 @@
   </si>
   <si>
     <t>U.K., 2017. The annual electoral register canvass in the cities of Hackney and Hull. 226,528 households.</t>
+  </si>
+  <si>
+    <t>Compared to registered voters as a whole, subjects who registered because of the treatment were more likely to be immigrants (+0.202, p&lt;0.01); born in another region of France (+0.215, p&lt;0.01); or young (age coefficient -0.137, p&lt;0.01). \newline \newline
+Voters registered from the treatments had higher turnout in the more salient  presidential election.</t>
   </si>
 </sst>
 </file>
@@ -682,8 +682,8 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -722,7 +722,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
@@ -731,12 +731,12 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>63</v>
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="288" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="288.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="322.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -813,7 +813,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -822,15 +822,15 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -850,16 +850,16 @@
         <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
@@ -870,7 +870,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -887,10 +887,10 @@
     </row>
     <row r="11" spans="1:6" ht="380" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -899,15 +899,15 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="256" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
@@ -924,7 +924,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -941,7 +941,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
@@ -950,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>31</v>
@@ -967,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="176" x14ac:dyDescent="0.2">
@@ -975,7 +975,7 @@
         <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -984,7 +984,7 @@
         <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>34</v>
@@ -995,7 +995,7 @@
         <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="18" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>38</v>

</xml_diff>